<commit_message>
updated board with test scenarios
</commit_message>
<xml_diff>
--- a/Clue Board.xlsx
+++ b/Clue Board.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="40">
   <si>
     <t>X</t>
   </si>
@@ -115,6 +115,27 @@
   </si>
   <si>
     <t>RU</t>
+  </si>
+  <si>
+    <t>Number of doors: 13</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in BoardInit Tests)</t>
+  </si>
+  <si>
+    <t>Orange: adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Yellow: adjaceny list tests, room exts</t>
+  </si>
+  <si>
+    <t>Gray: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Dark Purple: walkway scenarios</t>
+  </si>
+  <si>
+    <t>Dark Blue: test targets</t>
   </si>
 </sst>
 </file>
@@ -138,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +190,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,15 +239,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,19 +572,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -528,16 +593,16 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -546,16 +611,16 @@
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -564,16 +629,16 @@
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="5" t="s">
+      <c r="T1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X1">
@@ -581,34 +646,34 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -617,61 +682,61 @@
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="5" t="s">
+      <c r="S2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="4"/>
+      <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -680,16 +745,16 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -698,16 +763,16 @@
       <c r="M3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -716,16 +781,16 @@
       <c r="S3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W3" s="5" t="s">
+      <c r="T3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X3">
@@ -739,19 +804,19 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -760,16 +825,16 @@
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -778,16 +843,16 @@
       <c r="M4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -796,16 +861,16 @@
       <c r="S4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="5" t="s">
+      <c r="T4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X4">
@@ -819,19 +884,19 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -840,16 +905,16 @@
       <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -858,16 +923,16 @@
       <c r="M5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -876,25 +941,25 @@
       <c r="S5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W5" s="5" t="s">
+      <c r="T5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X5">
         <v>4</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AA5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -941,13 +1006,13 @@
       <c r="N6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="5" t="s">
+      <c r="O6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -956,25 +1021,25 @@
       <c r="S6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="5" t="s">
+      <c r="T6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X6">
         <v>5</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AA6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1000,7 +1065,7 @@
       <c r="G7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="13" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1033,48 +1098,48 @@
       <c r="R7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W7" s="5" t="s">
+      <c r="U7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X7">
         <v>6</v>
       </c>
-      <c r="Z7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA7" s="5" t="s">
+      <c r="Z7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1116,45 +1181,45 @@
       <c r="S8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="U8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="5" t="s">
+      <c r="U8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X8">
         <v>7</v>
       </c>
-      <c r="Z8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA8" s="5" t="s">
+      <c r="Z8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1187,57 +1252,57 @@
       <c r="P9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W9" s="5" t="s">
+      <c r="Q9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X9">
         <v>8</v>
       </c>
-      <c r="Z9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA9" s="5" t="s">
+      <c r="Z9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1267,54 +1332,54 @@
       <c r="P10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W10" s="5" t="s">
+      <c r="Q10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="X10">
         <v>9</v>
       </c>
-      <c r="Z10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA10" s="5" t="s">
+      <c r="Z10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1356,7 +1421,7 @@
       <c r="S11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="13" t="s">
         <v>2</v>
       </c>
       <c r="U11" s="1" t="s">
@@ -1371,30 +1436,30 @@
       <c r="X11">
         <v>10</v>
       </c>
-      <c r="Z11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA11" s="5" t="s">
+      <c r="Z11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1451,30 +1516,30 @@
       <c r="X12">
         <v>11</v>
       </c>
-      <c r="Z12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA12" s="5" t="s">
+      <c r="Z12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1507,54 +1572,54 @@
       <c r="P13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="W13" s="5" t="s">
+      <c r="Q13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="X13">
         <v>12</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="Z13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AA13" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1584,28 +1649,28 @@
       <c r="O14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="2" t="s">
+      <c r="P14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="V14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="W14" s="5" t="s">
+      <c r="R14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="X14">
@@ -1617,22 +1682,22 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1656,7 +1721,7 @@
       <c r="M15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="N15" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O15" s="1" t="s">
@@ -1665,25 +1730,25 @@
       <c r="P15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="W15" s="5" t="s">
+      <c r="Q15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="X15">
@@ -1715,22 +1780,22 @@
       <c r="H16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="5" t="s">
+      <c r="I16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -1739,25 +1804,25 @@
       <c r="P16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="W16" s="5" t="s">
+      <c r="Q16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="X16">
@@ -1768,7 +1833,7 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1789,22 +1854,22 @@
       <c r="H17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="5" t="s">
+      <c r="I17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -1839,19 +1904,19 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1866,19 +1931,19 @@
       <c r="I18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18" s="5" t="s">
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O18" s="1" t="s">
@@ -1896,7 +1961,7 @@
       <c r="S18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="10" t="s">
         <v>2</v>
       </c>
       <c r="U18" s="1" t="s">
@@ -1905,7 +1970,7 @@
       <c r="V18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="W18" s="11" t="s">
         <v>2</v>
       </c>
       <c r="X18">
@@ -1913,19 +1978,19 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="A19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1937,22 +2002,22 @@
       <c r="H19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="5" t="s">
+      <c r="J19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O19" s="1" t="s">
@@ -1961,25 +2026,25 @@
       <c r="P19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T19" s="2" t="s">
+      <c r="Q19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W19" s="5" t="s">
+      <c r="U19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X19">
@@ -1987,19 +2052,19 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -2008,25 +2073,25 @@
       <c r="G20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="5" t="s">
+      <c r="H20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O20" s="1" t="s">
@@ -2035,25 +2100,25 @@
       <c r="P20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W20" s="5" t="s">
+      <c r="Q20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X20">
@@ -2061,19 +2126,19 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2082,25 +2147,25 @@
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N21" s="5" t="s">
+      <c r="H21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -2109,25 +2174,25 @@
       <c r="P21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W21" s="5" t="s">
+      <c r="Q21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X21">
@@ -2135,19 +2200,19 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2156,25 +2221,25 @@
       <c r="G22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="5" t="s">
+      <c r="H22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O22" s="1" t="s">
@@ -2183,25 +2248,25 @@
       <c r="P22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W22" s="5" t="s">
+      <c r="Q22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X22">
@@ -2209,19 +2274,19 @@
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="A23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2230,52 +2295,52 @@
       <c r="G23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N23" s="5" t="s">
+      <c r="H23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W23" s="5" t="s">
+      <c r="P23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X23">
@@ -2353,9 +2418,118 @@
         <v>22</v>
       </c>
     </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A27:N27"/>
     <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A30:M30"/>
+    <mergeCell ref="A31:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Failed tests written for adjacency. Changed file for tests.
</commit_message>
<xml_diff>
--- a/Clue Board.xlsx
+++ b/Clue Board.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="39">
   <si>
     <t>X</t>
   </si>
@@ -120,22 +120,19 @@
     <t>Number of doors: 13</t>
   </si>
   <si>
-    <t>White: door direction tests (in BoardInit Tests)</t>
-  </si>
-  <si>
-    <t>Orange: adjacency list tests, inside room</t>
-  </si>
-  <si>
-    <t>Yellow: adjaceny list tests, room exts</t>
-  </si>
-  <si>
-    <t>Gray: adjacency lists beside room entrance</t>
-  </si>
-  <si>
-    <t>Dark Purple: walkway scenarios</t>
-  </si>
-  <si>
-    <t>Dark Blue: test targets</t>
+    <t>Dark Purple: walkway scenarios and edge cases</t>
+  </si>
+  <si>
+    <t>Green: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Red: adjacency next to rooms</t>
+  </si>
+  <si>
+    <t>Yellow: adjaceny list tests, room exits</t>
+  </si>
+  <si>
+    <t>Orange: test targets</t>
   </si>
 </sst>
 </file>
@@ -222,7 +219,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.499984740745262"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,22 +236,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -557,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +642,7 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -664,7 +660,7 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -682,7 +678,7 @@
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N2" s="4" t="s">
@@ -700,7 +696,7 @@
       <c r="R2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -718,10 +714,10 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="5"/>
+      <c r="AA2" s="10"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -804,7 +800,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -816,7 +812,7 @@
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -884,7 +880,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -896,7 +892,7 @@
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -923,7 +919,7 @@
       <c r="M5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="O5" s="4" t="s">
@@ -1006,7 +1002,7 @@
       <c r="N6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="4" t="s">
@@ -1065,7 +1061,7 @@
       <c r="G7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1098,7 +1094,7 @@
       <c r="R7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="S7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="T7" s="2" t="s">
@@ -1181,7 +1177,7 @@
       <c r="S8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="U8" s="4" t="s">
@@ -1302,7 +1298,7 @@
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1329,7 +1325,7 @@
       <c r="O10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="12" t="s">
         <v>2</v>
       </c>
       <c r="Q10" s="4" t="s">
@@ -1379,7 +1375,7 @@
       <c r="E11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1421,7 +1417,7 @@
       <c r="S11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="13" t="s">
+      <c r="T11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="U11" s="1" t="s">
@@ -1459,10 +1455,10 @@
       <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1649,10 +1645,10 @@
       <c r="O14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="6" t="s">
+      <c r="P14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="R14" s="4" t="s">
@@ -1700,7 +1696,7 @@
       <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1721,7 +1717,7 @@
       <c r="M15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N15" s="13" t="s">
+      <c r="N15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="O15" s="1" t="s">
@@ -1730,7 +1726,7 @@
       <c r="P15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="Q15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="R15" s="4" t="s">
@@ -1795,7 +1791,7 @@
       <c r="M16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -1833,7 +1829,7 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1910,10 +1906,10 @@
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1961,7 +1957,7 @@
       <c r="S18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="6" t="s">
         <v>2</v>
       </c>
       <c r="U18" s="1" t="s">
@@ -1970,7 +1966,7 @@
       <c r="V18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="W18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="X18">
@@ -2002,7 +1998,7 @@
       <c r="H19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J19" s="4" t="s">
@@ -2035,13 +2031,13 @@
       <c r="S19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="V19" s="9" t="s">
+      <c r="V19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="W19" s="4" t="s">
@@ -2082,7 +2078,7 @@
       <c r="J20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L20" s="4" t="s">
@@ -2316,10 +2312,10 @@
       <c r="N23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P23" s="11" t="s">
+      <c r="O23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="7" t="s">
         <v>2</v>
       </c>
       <c r="Q23" s="4" t="s">
@@ -2419,117 +2415,99 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A27:N27"/>
+  <mergeCells count="7">
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A30:G30"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="A30:M30"/>
-    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>